<commit_message>
Historias de Usuario Evaluación Docente
</commit_message>
<xml_diff>
--- a/HU_EvaluacionDocente.xlsx
+++ b/HU_EvaluacionDocente.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\Universidad\9no Semestre\Arquitectura de Software\II Parcial\UniversidadDocs\UniversidadDocs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\Universidad\9no Semestre\Arquitectura de Software\II Parcial\UniversidadDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,9 +26,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="62">
   <si>
-    <t>Desarrollo ágil: Historias de usuario y criterios de aceptación</t>
-  </si>
-  <si>
     <t>Enunciado de la historia</t>
   </si>
   <si>
@@ -44,9 +41,6 @@
     <t>Razón / Resultado</t>
   </si>
   <si>
-    <t>ED-02</t>
-  </si>
-  <si>
     <t>Como un Directivo/Administrador</t>
   </si>
   <si>
@@ -56,54 +50,36 @@
     <t xml:space="preserve">Con la finalidad de  corregir la/s evaluacion/es que se van a llevar a cabo en caso de contener un error. </t>
   </si>
   <si>
-    <t>ED-03</t>
-  </si>
-  <si>
     <t>Necesito crear cuestionarios de evaluación.</t>
   </si>
   <si>
     <t xml:space="preserve">Con la finalidad de  organizar las preguntas que formarán parte de las diferentes evaluaciones. </t>
   </si>
   <si>
-    <t>ED-04</t>
-  </si>
-  <si>
     <t>Necesito modificar cuestionarios de evaluación.</t>
   </si>
   <si>
     <t xml:space="preserve">Con la finalidad de que en caso de error, corregir que preguntas formarán parte de las diferentes evaluaciones. </t>
   </si>
   <si>
-    <t>ED-05</t>
-  </si>
-  <si>
     <t>Necesito crear preguntas de evaluación.</t>
   </si>
   <si>
     <t xml:space="preserve">Con la finalidad de conformar los cuestionarios de evaluación. </t>
   </si>
   <si>
-    <t>ED-06</t>
-  </si>
-  <si>
     <t>Necesito modificar preguntas de evaluación.</t>
   </si>
   <si>
     <t>Con la finalidad de  corregir las preguntas que contengan algun error.</t>
   </si>
   <si>
-    <t>ED-07</t>
-  </si>
-  <si>
     <t>Necesito asignar cuestionarios por rol y dar una ponderación a los mismos para cada evaluación.</t>
   </si>
   <si>
     <t xml:space="preserve">Con la finalidad de  establecer los detalles de evaluación. </t>
   </si>
   <si>
-    <t>ED-08</t>
-  </si>
-  <si>
     <t>Como un Estudiante</t>
   </si>
   <si>
@@ -113,27 +89,18 @@
     <t>Con la finalidad de  escoger el curso sobre el cual se va a realizar la evaluación.</t>
   </si>
   <si>
-    <t>ED-09</t>
-  </si>
-  <si>
     <t>Necesito poder seleccionar la respuesta a cada pregunta de la evaluación al docente del NRC seleccionado.</t>
   </si>
   <si>
     <t>Con la finalidad de  establecer la calificación de cada pregunta.</t>
   </si>
   <si>
-    <t>ED-10</t>
-  </si>
-  <si>
     <t>Necesito enviar el cuestionario respondido para que sea almacenado y procesado.</t>
   </si>
   <si>
     <t>Con la finalidad de almacenar las respuestas establecidas en cada una de las preguntas.</t>
   </si>
   <si>
-    <t>ED-11</t>
-  </si>
-  <si>
     <t>Como un Docente</t>
   </si>
   <si>
@@ -143,18 +110,9 @@
     <t>Con la finalidad de  escoger el NRC sobre el cual se va a realizar la autoevaluación.</t>
   </si>
   <si>
-    <t>ED-12</t>
-  </si>
-  <si>
     <t>Necesito poder seleccionar la respuesta a cada pregunta de la autoevaluación del NRC seleccionado.</t>
   </si>
   <si>
-    <t>ED-13</t>
-  </si>
-  <si>
-    <t>ED-14</t>
-  </si>
-  <si>
     <t>Como un Director</t>
   </si>
   <si>
@@ -164,45 +122,27 @@
     <t>Con la finalidad de  escoger el NRC sobre el cual se va a realizar la evaluación docente.</t>
   </si>
   <si>
-    <t>ED-15</t>
-  </si>
-  <si>
     <t>Necesito poder seleccionar la respuesta a cada pregunta de la evaluación del NRC seleccionado.</t>
   </si>
   <si>
-    <t>ED-16</t>
-  </si>
-  <si>
-    <t>ED-17</t>
-  </si>
-  <si>
     <t>Necesito visualizar el resultado promedio por NRC.</t>
   </si>
   <si>
     <t>Con la finalidad de apreciar una calificación goblal que se ha obtenido por NRC.</t>
   </si>
   <si>
-    <t>ED-18</t>
-  </si>
-  <si>
     <t>Necesito visualizar el resultado de cada docente por NRC asigando respectivamente.</t>
   </si>
   <si>
     <t>Con la finalidad de apreciar una calificación goblal que se ha obtenido por NRC de cada docete.</t>
   </si>
   <si>
-    <t>ED-19</t>
-  </si>
-  <si>
     <t>Necesito visualizar el resultado promedio global de cada docente.</t>
   </si>
   <si>
     <t>Con la finalidad de apreciar una calificación goblal que ha obtenido cada docente.</t>
   </si>
   <si>
-    <t>ED-20</t>
-  </si>
-  <si>
     <t>Como un Administrador</t>
   </si>
   <si>
@@ -210,6 +150,66 @@
   </si>
   <si>
     <t>Con la finalidad de obtener una calificación más exacta del desepeño del docente.</t>
+  </si>
+  <si>
+    <t>Desarrollo ágil: Historias de usuario y criterios de aceptación - Evaluación Docente</t>
+  </si>
+  <si>
+    <t>UN-EVA-01</t>
+  </si>
+  <si>
+    <t>UN-EVA-02</t>
+  </si>
+  <si>
+    <t>UN-EVA-03</t>
+  </si>
+  <si>
+    <t>UN-EVA-04</t>
+  </si>
+  <si>
+    <t>UN-EVA-05</t>
+  </si>
+  <si>
+    <t>UN-EVA-06</t>
+  </si>
+  <si>
+    <t>UN-EVA-07</t>
+  </si>
+  <si>
+    <t>UN-EVA-08</t>
+  </si>
+  <si>
+    <t>UN-EVA-09</t>
+  </si>
+  <si>
+    <t>UN-EVA-10</t>
+  </si>
+  <si>
+    <t>UN-EVA-11</t>
+  </si>
+  <si>
+    <t>UN-EVA-12</t>
+  </si>
+  <si>
+    <t>UN-EVA-13</t>
+  </si>
+  <si>
+    <t>UN-EVA-14</t>
+  </si>
+  <si>
+    <t>UN-EVA-15</t>
+  </si>
+  <si>
+    <t>UN-EVA-16</t>
+  </si>
+  <si>
+    <t>UN-EVA-17</t>
+  </si>
+  <si>
+    <t>UN-EVA-18</t>
+  </si>
+  <si>
+    <t>UN-EVA-19</t>
   </si>
 </sst>
 </file>
@@ -316,8 +316,6 @@
   </cellStyleXfs>
   <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -343,6 +341,8 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -629,10 +629,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="B3:E45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D52" sqref="D52"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -644,419 +647,419 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:5" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B6" s="2"/>
+      <c r="C6" s="14" t="s">
         <v>0</v>
-      </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B6" s="4"/>
-      <c r="C6" s="14" t="s">
-        <v>1</v>
       </c>
       <c r="D6" s="15"/>
       <c r="E6" s="15"/>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="D7" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="E7" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="6" t="s">
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B8" s="5"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+    </row>
+    <row r="9" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B9" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" s="8" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B8" s="7"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-    </row>
-    <row r="9" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B9" s="9" t="s">
+      <c r="D9" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="E9" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="10" t="s">
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B10" s="5"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+    </row>
+    <row r="11" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B11" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="E11" s="8" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B10" s="7"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-    </row>
-    <row r="11" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B11" s="9" t="s">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B12" s="5"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+    </row>
+    <row r="13" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B13" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" s="10" t="s">
+      <c r="E13" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E11" s="10" t="s">
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B14" s="5"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+    </row>
+    <row r="15" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B15" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="8" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B12" s="7"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-    </row>
-    <row r="13" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B13" s="9" t="s">
+      <c r="E15" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13" s="10" t="s">
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B16" s="5"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+    </row>
+    <row r="17" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B17" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="E17" s="8" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B14" s="7"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-    </row>
-    <row r="15" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B15" s="9" t="s">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B18" s="5"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+    </row>
+    <row r="19" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B19" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="D15" s="10" t="s">
+      <c r="E19" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="E15" s="10" t="s">
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B20" s="5"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+    </row>
+    <row r="21" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B21" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C21" s="8" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B16" s="7"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-    </row>
-    <row r="17" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B17" s="9" t="s">
+      <c r="D21" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="D17" s="10" t="s">
+      <c r="E21" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="E17" s="10" t="s">
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B22" s="5"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+    </row>
+    <row r="23" spans="2:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B23" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D23" s="9" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B18" s="7"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-    </row>
-    <row r="19" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B19" s="9" t="s">
+      <c r="E23" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C19" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="D19" s="10" t="s">
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B24" s="5"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+    </row>
+    <row r="25" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B25" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D25" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="E19" s="10" t="s">
+      <c r="E25" s="8" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B20" s="7"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-    </row>
-    <row r="21" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B21" s="9" t="s">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B26" s="5"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+    </row>
+    <row r="27" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B27" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C27" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C21" s="10" t="s">
+      <c r="D27" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="D21" s="10" t="s">
+      <c r="E27" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E21" s="10" t="s">
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B28" s="5"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+    </row>
+    <row r="29" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B29" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D29" s="9" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B22" s="7"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
-    </row>
-    <row r="23" spans="2:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B23" s="9" t="s">
+      <c r="E29" s="9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B30" s="5"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+    </row>
+    <row r="31" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B31" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E31" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B32" s="5"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
+    </row>
+    <row r="33" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B33" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C33" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C23" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="D23" s="11" t="s">
+      <c r="D33" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="E23" s="11" t="s">
+      <c r="E33" s="8" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B24" s="7"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="8"/>
-    </row>
-    <row r="25" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B25" s="9" t="s">
+    <row r="34" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B34" s="5"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
+    </row>
+    <row r="35" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B35" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D35" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="C25" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="D25" s="10" t="s">
+      <c r="E35" s="9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B36" s="5"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="6"/>
+    </row>
+    <row r="37" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B37" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D37" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E37" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B38" s="5"/>
+      <c r="C38" s="6"/>
+      <c r="D38" s="6"/>
+      <c r="E38" s="6"/>
+    </row>
+    <row r="39" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B39" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="C39" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D39" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="E25" s="10" t="s">
+      <c r="E39" s="11" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B26" s="7"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="8"/>
-    </row>
-    <row r="27" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B27" s="9" t="s">
+    <row r="40" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B40" s="5"/>
+      <c r="C40" s="6"/>
+      <c r="D40" s="6"/>
+      <c r="E40" s="6"/>
+    </row>
+    <row r="41" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B41" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="C41" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D41" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="C27" s="10" t="s">
+      <c r="E41" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="D27" s="10" t="s">
+    </row>
+    <row r="42" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B42" s="5"/>
+      <c r="C42" s="6"/>
+      <c r="D42" s="6"/>
+      <c r="E42" s="6"/>
+    </row>
+    <row r="43" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B43" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="C43" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D43" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="E27" s="10" t="s">
+      <c r="E43" s="11" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B28" s="7"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="8"/>
-      <c r="E28" s="8"/>
-    </row>
-    <row r="29" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B29" s="9" t="s">
+    <row r="44" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B44" s="5"/>
+      <c r="C44" s="6"/>
+      <c r="D44" s="6"/>
+      <c r="E44" s="6"/>
+    </row>
+    <row r="45" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B45" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="C45" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="C29" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="D29" s="11" t="s">
+      <c r="D45" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="E29" s="11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B30" s="7"/>
-      <c r="C30" s="8"/>
-      <c r="D30" s="8"/>
-      <c r="E30" s="8"/>
-    </row>
-    <row r="31" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B31" s="9" t="s">
+      <c r="E45" s="11" t="s">
         <v>41</v>
-      </c>
-      <c r="C31" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="D31" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="E31" s="10" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B32" s="7"/>
-      <c r="C32" s="8"/>
-      <c r="D32" s="8"/>
-      <c r="E32" s="8"/>
-    </row>
-    <row r="33" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B33" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="C33" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="D33" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="E33" s="10" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B34" s="7"/>
-      <c r="C34" s="8"/>
-      <c r="D34" s="8"/>
-      <c r="E34" s="8"/>
-    </row>
-    <row r="35" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B35" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="C35" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="D35" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="E35" s="11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B36" s="7"/>
-      <c r="C36" s="8"/>
-      <c r="D36" s="8"/>
-      <c r="E36" s="8"/>
-    </row>
-    <row r="37" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B37" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="C37" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="D37" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="E37" s="10" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B38" s="7"/>
-      <c r="C38" s="8"/>
-      <c r="D38" s="8"/>
-      <c r="E38" s="8"/>
-    </row>
-    <row r="39" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B39" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="C39" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="D39" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="E39" s="13" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B40" s="7"/>
-      <c r="C40" s="8"/>
-      <c r="D40" s="8"/>
-      <c r="E40" s="8"/>
-    </row>
-    <row r="41" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B41" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="C41" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="D41" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="E41" s="13" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B42" s="7"/>
-      <c r="C42" s="8"/>
-      <c r="D42" s="8"/>
-      <c r="E42" s="8"/>
-    </row>
-    <row r="43" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B43" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="C43" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="D43" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="E43" s="13" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B44" s="7"/>
-      <c r="C44" s="8"/>
-      <c r="D44" s="8"/>
-      <c r="E44" s="8"/>
-    </row>
-    <row r="45" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B45" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="C45" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="D45" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="E45" s="13" t="s">
-        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1065,5 +1068,6 @@
     <mergeCell ref="C6:E6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="58" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>